<commit_message>
Actualizacion de Backlog User
</commit_message>
<xml_diff>
--- a/Sprint backlog.xlsx
+++ b/Sprint backlog.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Datos\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211B0839-1406-4121-B24E-98AA61D59AFA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
   <si>
     <t>Identificador (ID) de item de product backlog</t>
   </si>
@@ -48,9 +47,6 @@
     <t>Descripción</t>
   </si>
   <si>
-    <t>00-0000-0001</t>
-  </si>
-  <si>
     <t>Responsable</t>
   </si>
   <si>
@@ -58,12 +54,6 @@
   </si>
   <si>
     <t>00-0000-0002</t>
-  </si>
-  <si>
-    <t>Como vecino quiero registrar un producto e ingresar la cantidad a reciclar, para actualizar mis estadísticas y reciclar el producto</t>
-  </si>
-  <si>
-    <t>Como vecino quiero ver las estadísticas de lo reciclado, para informarme sobre todo lo que reciclo</t>
   </si>
   <si>
     <t>Como vecino quiero conocer los datos sobre los puntos de recolección, para saber cuándo y dónde llevar mis productos</t>
@@ -183,31 +173,31 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Empleado Municipal               </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-  </si>
-  <si>
     <t>To do</t>
   </si>
   <si>
     <t>Empleado de  PL</t>
+  </si>
+  <si>
+    <t>US 1</t>
+  </si>
+  <si>
+    <t>Definicion, criterio de aceptacion, tareas</t>
+  </si>
+  <si>
+    <t>JJFMM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empleado Municipal               </t>
+  </si>
+  <si>
+    <t>Como vecino quiero registrar un producto e ingresar la cantidad a reciclar, para actualizar mis estadísticas y reciclar el producto shhgshghsghgshgshgshgshgs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -475,30 +465,54 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -517,9 +531,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -528,24 +539,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -555,9 +548,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -838,11 +828,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:K28"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -859,52 +849,52 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
     </row>
     <row r="2" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
     </row>
     <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
@@ -913,501 +903,512 @@
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43"/>
       <c r="H5" s="12" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
+        <v>6</v>
+      </c>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="14"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="26"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="34"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
     </row>
     <row r="7" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="37"/>
+      <c r="C7" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="19"/>
       <c r="H7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+    </row>
+    <row r="8" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-    </row>
-    <row r="8" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="B8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="37"/>
+      <c r="C8" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="19"/>
       <c r="H8" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
+        <v>7</v>
+      </c>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
     </row>
     <row r="9" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="37"/>
+      <c r="C9" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
       <c r="H9" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
+        <v>7</v>
+      </c>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
     </row>
     <row r="10" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="37"/>
+      <c r="C10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="19"/>
       <c r="H10" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
+        <v>7</v>
+      </c>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
     </row>
     <row r="11" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="37"/>
+      <c r="C11" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="19"/>
       <c r="H11" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
+        <v>7</v>
+      </c>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
     </row>
     <row r="12" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="20"/>
+      <c r="C12" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="25"/>
       <c r="H12" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
+        <v>7</v>
+      </c>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
     </row>
     <row r="13" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="37"/>
+      <c r="C13" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="19"/>
       <c r="H13" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
+        <v>7</v>
+      </c>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
     </row>
     <row r="14" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="37"/>
+      <c r="C14" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="19"/>
       <c r="H14" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
+        <v>7</v>
+      </c>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
     </row>
     <row r="15" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="37"/>
+      <c r="C15" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="19"/>
       <c r="H15" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
+        <v>45</v>
+      </c>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
     </row>
     <row r="16" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="37"/>
+      <c r="C16" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
+        <v>45</v>
+      </c>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
     </row>
     <row r="17" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="29"/>
+      <c r="C17" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="37"/>
       <c r="H17" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="I17" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
+        <v>44</v>
+      </c>
+      <c r="I17" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
     </row>
     <row r="18" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="7"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="32"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="39"/>
       <c r="H18" s="7"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
     </row>
     <row r="19" spans="1:17" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="23"/>
+      <c r="C19" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="22"/>
       <c r="H19" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
+        <v>45</v>
+      </c>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
     </row>
     <row r="20" spans="1:17" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="20"/>
+      <c r="C20" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="25"/>
       <c r="H20" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
+        <v>20</v>
+      </c>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
     </row>
     <row r="21" spans="1:17" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="20"/>
+      <c r="C21" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="25"/>
       <c r="H21" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="34"/>
-      <c r="P21" s="34"/>
-      <c r="Q21" s="34"/>
+        <v>20</v>
+      </c>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
     </row>
     <row r="22" spans="1:17" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="20"/>
+      <c r="C22" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="25"/>
       <c r="H22" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
+        <v>23</v>
+      </c>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
       <c r="M22" s="8"/>
       <c r="P22" s="8"/>
     </row>
     <row r="23" spans="1:17" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="20"/>
+      <c r="C23" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="25"/>
       <c r="H23" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
+        <v>23</v>
+      </c>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
     </row>
     <row r="24" spans="1:17" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="23"/>
+      <c r="C24" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="22"/>
       <c r="H24" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-    </row>
-    <row r="25" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+    </row>
+    <row r="25" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="20"/>
+      <c r="C25" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="25"/>
       <c r="H25" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
+        <v>49</v>
+      </c>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
+      <c r="A26" s="40"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="31"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="E1:K3"/>
+    <mergeCell ref="J4:K28"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="C17:G18"/>
+    <mergeCell ref="A26:I27"/>
+    <mergeCell ref="C5:G5"/>
     <mergeCell ref="M21:Q21"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C19:G19"/>
@@ -1423,19 +1424,8 @@
     <mergeCell ref="C15:G15"/>
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="C12:G12"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="E1:K3"/>
-    <mergeCell ref="J4:K28"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="C17:G18"/>
-    <mergeCell ref="A26:I27"/>
-    <mergeCell ref="C5:G5"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="85" fitToWidth="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>